<commit_message>
15 January 2024 - Added random data points to the two new variables.
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10107"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D36EA3-6DA7-DF4F-95A4-93AFDE92C5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F0B1FE-0209-434C-8D34-B1D69410721E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27300" yWindow="5760" windowWidth="48840" windowHeight="21640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26960" yWindow="8300" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
   <si>
     <t>Height</t>
   </si>
@@ -78,6 +78,18 @@
   </si>
   <si>
     <t>Political Party</t>
+  </si>
+  <si>
+    <t>Republican</t>
+  </si>
+  <si>
+    <t>Democrat</t>
+  </si>
+  <si>
+    <t>Libertarian</t>
+  </si>
+  <si>
+    <t>Green</t>
   </si>
 </sst>
 </file>
@@ -407,7 +419,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -439,6 +451,12 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
+      <c r="D2">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -450,6 +468,12 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
+      <c r="D3">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -461,6 +485,12 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
+      <c r="D4">
+        <v>89</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -472,6 +502,12 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
+      <c r="D5">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -483,6 +519,12 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
+      <c r="D6">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -494,6 +536,12 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
+      <c r="D7">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -505,6 +553,12 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
+      <c r="D8">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -516,6 +570,12 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -527,6 +587,12 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
+      <c r="D10">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -538,6 +604,12 @@
       <c r="C11" t="s">
         <v>3</v>
       </c>
+      <c r="D11">
+        <v>99</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -546,6 +618,12 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
+      <c r="D12">
+        <v>26</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -557,6 +635,12 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
+      <c r="D13">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -568,6 +652,12 @@
       <c r="C14" t="s">
         <v>3</v>
       </c>
+      <c r="D14">
+        <v>77</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -578,6 +668,12 @@
       </c>
       <c r="C15" t="s">
         <v>3</v>
+      </c>
+      <c r="D15">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
16 Jan 2024 Update - Added new variables to codebook
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10107"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F0B1FE-0209-434C-8D34-B1D69410721E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C7D39A-6C36-434F-BB5C-A43884553119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26960" yWindow="8300" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15840" yWindow="900" windowWidth="48360" windowHeight="27680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Height</t>
   </si>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t>Green</t>
+  </si>
+  <si>
+    <t>Age in years</t>
+  </si>
+  <si>
+    <t>Political party</t>
+  </si>
+  <si>
+    <t>Political party affiliation (categorical)</t>
+  </si>
+  <si>
+    <t>Republican/Democrat/Libertarian/Green/NA</t>
   </si>
 </sst>
 </file>
@@ -418,7 +430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -683,10 +695,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -740,6 +752,28 @@
         <v>14</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Recharacterized Political party variable into "Party" and reformulated into factor variable rather than character. 18 Jan 2024
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10107"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C7D39A-6C36-434F-BB5C-A43884553119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E3423A-CA89-DB48-8D1D-708F58615F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15840" yWindow="900" windowWidth="48360" windowHeight="27680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2840" yWindow="900" windowWidth="48360" windowHeight="27680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="26">
   <si>
     <t>Height</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Political Party</t>
-  </si>
-  <si>
     <t>Republican</t>
   </si>
   <si>
@@ -95,13 +92,13 @@
     <t>Age in years</t>
   </si>
   <si>
-    <t>Political party</t>
-  </si>
-  <si>
     <t>Political party affiliation (categorical)</t>
   </si>
   <si>
     <t>Republican/Democrat/Libertarian/Green/NA</t>
+  </si>
+  <si>
+    <t>Party</t>
   </si>
 </sst>
 </file>
@@ -430,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -450,7 +447,7 @@
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -467,7 +464,7 @@
         <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -484,7 +481,7 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -501,7 +498,7 @@
         <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -518,7 +515,7 @@
         <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -535,7 +532,7 @@
         <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -552,7 +549,7 @@
         <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -569,7 +566,7 @@
         <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -586,7 +583,7 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -603,7 +600,7 @@
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -620,7 +617,7 @@
         <v>99</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -634,7 +631,7 @@
         <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -651,7 +648,7 @@
         <v>56</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -668,7 +665,7 @@
         <v>77</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -685,7 +682,7 @@
         <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -697,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -757,7 +754,7 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -765,13 +762,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>